<commit_message>
New nakshatra query tool based on lordships bug free :)
</commit_message>
<xml_diff>
--- a/script_to_gen_horoscope_and_stor/dataset/Ashwin Anna.xlsx
+++ b/script_to_gen_horoscope_and_stor/dataset/Ashwin Anna.xlsx
@@ -461,7 +461,7 @@
       </c>
       <c r="B4" t="inlineStr">
         <is>
-          <t>07:34:00</t>
+          <t>19:34:00</t>
         </is>
       </c>
     </row>
@@ -473,7 +473,7 @@
       </c>
       <c r="B5" t="inlineStr">
         <is>
-          <t>Moodabidri,Karnataka</t>
+          <t>Bantwal,Karnataka</t>
         </is>
       </c>
     </row>
@@ -484,7 +484,7 @@
         </is>
       </c>
       <c r="B6" t="n">
-        <v>13.0699218</v>
+        <v>12.8953789</v>
       </c>
     </row>
     <row r="7">
@@ -494,7 +494,7 @@
         </is>
       </c>
       <c r="B7" t="n">
-        <v>74.9977469</v>
+        <v>75.0408618</v>
       </c>
     </row>
     <row r="8">
@@ -639,26 +639,26 @@
       </c>
       <c r="B3" t="inlineStr">
         <is>
-          <t>Capricorn</t>
+          <t>Leo</t>
         </is>
       </c>
       <c r="C3" t="inlineStr">
         <is>
-          <t>Saturn</t>
+          <t>Sun</t>
         </is>
       </c>
       <c r="D3" t="inlineStr">
         <is>
-          <t>Dhanishta</t>
+          <t>Magha</t>
         </is>
       </c>
       <c r="E3" t="inlineStr">
         <is>
-          <t>Mars</t>
+          <t>Ketu</t>
         </is>
       </c>
       <c r="F3" t="n">
-        <v>25.57069578701595</v>
+        <v>2.818248223016099</v>
       </c>
       <c r="G3" t="inlineStr">
         <is>
@@ -711,7 +711,7 @@
         </is>
       </c>
       <c r="F4" t="n">
-        <v>286.4335708475888</v>
+        <v>286.9412862534865</v>
       </c>
       <c r="G4" t="inlineStr">
         <is>
@@ -729,7 +729,7 @@
         </is>
       </c>
       <c r="J4" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K4" t="inlineStr">
         <is>
@@ -764,7 +764,7 @@
         </is>
       </c>
       <c r="F5" t="n">
-        <v>6.463896469000333</v>
+        <v>12.57328065113894</v>
       </c>
       <c r="G5" t="inlineStr">
         <is>
@@ -782,7 +782,7 @@
         </is>
       </c>
       <c r="J5" t="n">
-        <v>4</v>
+        <v>9</v>
       </c>
       <c r="K5" t="inlineStr">
         <is>
@@ -817,7 +817,7 @@
         </is>
       </c>
       <c r="F6" t="n">
-        <v>290.976381857157</v>
+        <v>291.8539258992433</v>
       </c>
       <c r="G6" t="inlineStr">
         <is>
@@ -835,7 +835,7 @@
         </is>
       </c>
       <c r="J6" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K6" t="inlineStr">
         <is>
@@ -861,16 +861,16 @@
       </c>
       <c r="D7" t="inlineStr">
         <is>
-          <t>Purva Bhadrapada</t>
+          <t>Uttara Bhadrapada</t>
         </is>
       </c>
       <c r="E7" t="inlineStr">
         <is>
-          <t>Jupiter</t>
+          <t>Saturn</t>
         </is>
       </c>
       <c r="F7" t="n">
-        <v>333.0905404744483</v>
+        <v>333.5552974085365</v>
       </c>
       <c r="G7" t="inlineStr">
         <is>
@@ -888,7 +888,7 @@
         </is>
       </c>
       <c r="J7" t="n">
-        <v>3</v>
+        <v>8</v>
       </c>
       <c r="K7" t="inlineStr">
         <is>
@@ -923,7 +923,7 @@
         </is>
       </c>
       <c r="F8" t="n">
-        <v>76.62372784919866</v>
+        <v>76.51867948886958</v>
       </c>
       <c r="G8" t="inlineStr">
         <is>
@@ -941,7 +941,7 @@
         </is>
       </c>
       <c r="J8" t="n">
-        <v>6</v>
+        <v>11</v>
       </c>
       <c r="K8" t="inlineStr">
         <is>
@@ -976,7 +976,7 @@
         </is>
       </c>
       <c r="F9" t="n">
-        <v>170.9283821823207</v>
+        <v>170.9261886981888</v>
       </c>
       <c r="G9" t="inlineStr">
         <is>
@@ -994,7 +994,7 @@
         </is>
       </c>
       <c r="J9" t="n">
-        <v>9</v>
+        <v>2</v>
       </c>
       <c r="K9" t="inlineStr">
         <is>
@@ -1029,7 +1029,7 @@
         </is>
       </c>
       <c r="F10" t="n">
-        <v>295.8931414435939</v>
+        <v>295.952888004387</v>
       </c>
       <c r="G10" t="inlineStr">
         <is>
@@ -1047,7 +1047,7 @@
         </is>
       </c>
       <c r="J10" t="n">
-        <v>1</v>
+        <v>6</v>
       </c>
       <c r="K10" t="inlineStr">
         <is>
@@ -1082,7 +1082,7 @@
         </is>
       </c>
       <c r="F11" t="n">
-        <v>265.6129809352763</v>
+        <v>265.6412131325364</v>
       </c>
       <c r="G11" t="inlineStr">
         <is>
@@ -1100,7 +1100,7 @@
         </is>
       </c>
       <c r="J11" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K11" t="inlineStr">
         <is>
@@ -1135,7 +1135,7 @@
         </is>
       </c>
       <c r="F12" t="n">
-        <v>265.6795242402326</v>
+        <v>265.6974764303666</v>
       </c>
       <c r="G12" t="inlineStr">
         <is>
@@ -1153,7 +1153,7 @@
         </is>
       </c>
       <c r="J12" t="n">
-        <v>12</v>
+        <v>5</v>
       </c>
       <c r="K12" t="inlineStr">
         <is>
@@ -1188,7 +1188,7 @@
         </is>
       </c>
       <c r="F13" t="n">
-        <v>211.5318931493858</v>
+        <v>211.5399106679366</v>
       </c>
       <c r="G13" t="inlineStr">
         <is>
@@ -1206,7 +1206,7 @@
         </is>
       </c>
       <c r="J13" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K13" t="inlineStr">
         <is>
@@ -1241,7 +1241,7 @@
         </is>
       </c>
       <c r="F14" t="n">
-        <v>235.1201795863594</v>
+        <v>235.0936835767791</v>
       </c>
       <c r="G14" t="inlineStr">
         <is>
@@ -1259,7 +1259,7 @@
         </is>
       </c>
       <c r="J14" t="n">
-        <v>11</v>
+        <v>4</v>
       </c>
       <c r="K14" t="inlineStr">
         <is>
@@ -1294,7 +1294,7 @@
         </is>
       </c>
       <c r="F15" t="n">
-        <v>55.12017958635937</v>
+        <v>55.09368357677914</v>
       </c>
       <c r="G15" t="inlineStr">
         <is>
@@ -1312,7 +1312,7 @@
         </is>
       </c>
       <c r="J15" t="n">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="K15" t="inlineStr">
         <is>

</xml_diff>